<commit_message>
Regione: REGIONE_CAMPANIA, Issuer: integrity:S1#190201234567XX
</commit_message>
<xml_diff>
--- a/REGIONE_CAMPANIA/integrity:S1#190201234567XX.xlsx
+++ b/REGIONE_CAMPANIA/integrity:S1#190201234567XX.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -42,6 +42,15 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.110.4.4^UAT_GTW_ID1721126641364</t>
+  </si>
+  <si>
+    <t>Creazione_1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.82e982b6d7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4^UAT_GTW_ID1721127047639</t>
   </si>
 </sst>
 </file>
@@ -86,7 +95,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -126,6 +135,23 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>